<commit_message>
Gail's edits to abstract
git-svn-id: https://svn.mcs.anl.gov/repos/performance/orio@401 e7ad4b5f-b827-0410-872f-f7f4bc3d1efb
</commit_message>
<xml_diff>
--- a/doc/papers/iccs09/figures/experiments.xlsx
+++ b/doc/papers/iccs09/figures/experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-680" yWindow="-21520" windowWidth="28520" windowHeight="21000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="32660" windowHeight="20440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>C from Matlab</t>
   </si>
@@ -189,6 +189,10 @@
     <t>Orio (Par.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>BG/P (seconds)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -253,7 +257,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -283,9 +287,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -379,9 +380,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -475,9 +473,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -571,9 +566,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -667,9 +659,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -763,9 +752,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -846,25 +832,38 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="431788392"/>
-        <c:axId val="431791560"/>
+        <c:axId val="528458312"/>
+        <c:axId val="528461480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431788392"/>
+        <c:axId val="528458312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431791560"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528461480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431791560"/>
+        <c:axId val="528461480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +871,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431788392"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528458312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -883,31 +895,25 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.196076444316898"/>
-          <c:y val="0.0491971902073696"/>
-          <c:w val="0.707618258244035"/>
+          <c:x val="0.132295123132387"/>
+          <c:y val="0.0350938124483963"/>
+          <c:w val="0.812401843846968"/>
           <c:h val="0.151329532084352"/>
         </c:manualLayout>
       </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr>
-    <a:ln w="9525">
-      <a:prstDash val="sysDot"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200" baseline="0"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -921,7 +927,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -951,9 +957,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1047,9 +1050,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1143,9 +1143,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1239,9 +1236,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1335,9 +1329,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1431,9 +1422,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1514,25 +1502,38 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="431860792"/>
-        <c:axId val="431863960"/>
+        <c:axId val="656502760"/>
+        <c:axId val="656505928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431860792"/>
+        <c:axId val="656502760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431863960"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656505928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431863960"/>
+        <c:axId val="656505928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1541,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431860792"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656502760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1551,31 +1565,25 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.194483525550195"/>
-          <c:y val="0.0176660232512813"/>
-          <c:w val="0.707618258244035"/>
+          <c:x val="0.139813821677757"/>
+          <c:y val="0.0143074636978058"/>
+          <c:w val="0.821513461159041"/>
           <c:h val="0.14414966377378"/>
         </c:manualLayout>
       </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr>
-    <a:ln w="9525">
-      <a:prstDash val="sysDot"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200" baseline="0"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1589,7 +1597,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -1619,9 +1627,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -1715,9 +1720,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -1811,9 +1813,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -1907,9 +1906,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -2003,9 +1999,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -2099,9 +2092,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$46:$K$46</c:f>
@@ -2182,25 +2172,38 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="431908840"/>
-        <c:axId val="431912104"/>
+        <c:axId val="656576328"/>
+        <c:axId val="656564232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431908840"/>
+        <c:axId val="656576328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431912104"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656564232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431912104"/>
+        <c:axId val="656564232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2211,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431908840"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656576328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,31 +2235,25 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.173525729557154"/>
-          <c:y val="0.000305665726626566"/>
-          <c:w val="0.707618258244035"/>
+          <c:x val="0.149772757027699"/>
+          <c:y val="0.00671993454314041"/>
+          <c:w val="0.800650712900792"/>
           <c:h val="0.151329532084352"/>
         </c:manualLayout>
       </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr>
-    <a:ln w="9525">
-      <a:prstDash val="sysDot"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200" baseline="0"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2257,7 +2267,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -2287,9 +2297,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2383,9 +2390,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2479,9 +2483,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2575,9 +2576,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2671,9 +2669,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2767,9 +2762,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2850,25 +2842,38 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="431957032"/>
-        <c:axId val="431960232"/>
+        <c:axId val="656621240"/>
+        <c:axId val="656624568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431957032"/>
+        <c:axId val="656621240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431960232"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656624568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431960232"/>
+        <c:axId val="656624568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,7 +2881,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431957032"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656621240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2887,31 +2905,25 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17119094488189"/>
-          <c:y val="0.0222363653929762"/>
-          <c:w val="0.724945037810868"/>
+          <c:x val="0.151467020764416"/>
+          <c:y val="0.0222362709469009"/>
+          <c:w val="0.788061470126885"/>
           <c:h val="0.129857253272789"/>
         </c:manualLayout>
       </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr>
-    <a:ln w="9525">
-      <a:prstDash val="sysDot"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200" baseline="0"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2925,7 +2937,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -2933,10 +2945,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0982086918424223"/>
+          <c:x val="0.137919010123735"/>
           <c:y val="0.0263381928744055"/>
-          <c:w val="0.852568121797758"/>
-          <c:h val="0.841159663210416"/>
+          <c:w val="0.820822084739407"/>
+          <c:h val="0.741538485014954"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2955,9 +2967,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$102:$K$102</c:f>
@@ -3051,13 +3064,99 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$104:$K$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>695.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>834.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>984.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1003.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1151.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1150.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1154.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1153.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$105</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (Seq.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:spPr>
               <a:ln>
@@ -3108,106 +3207,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$104:$K$104</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>15.14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>122.53</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>695.77</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>834.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>984.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1003.73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1151.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1150.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1154.57</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1153.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$105</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ESSL (Seq.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:srgbClr val="00FF00"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$B$105:$K$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3239,9 +3238,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$102:$K$102</c:f>
@@ -3314,9 +3310,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$102:$K$102</c:f>
@@ -3389,9 +3382,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050"/>
-          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$102:$K$102</c:f>
@@ -3464,14 +3454,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FF00FF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
           <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
@@ -3573,18 +3558,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
           <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="13"/>
             <c:spPr>
-              <a:ln w="28575" cmpd="sng">
+              <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -3669,25 +3649,38 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="451534792"/>
-        <c:axId val="451537912"/>
+        <c:axId val="656689256"/>
+        <c:axId val="656694264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451534792"/>
+        <c:axId val="656689256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451537912"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656694264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451537912"/>
+        <c:axId val="656694264"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3696,9 +3689,22 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451534792"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656689256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3709,40 +3715,815 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.656237267095863"/>
-          <c:y val="0.599009900990099"/>
-          <c:w val="0.290159670922124"/>
+          <c:x val="0.533926696662917"/>
+          <c:y val="0.518260544466825"/>
+          <c:w val="0.404533704925215"/>
           <c:h val="0.228952989787168"/>
         </c:manualLayout>
       </c:layout>
-      <c:spPr>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:spPr>
-    <a:ln w="9525">
-      <a:prstDash val="sysDot"/>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
     </a:ln>
-    <a:effectLst/>
   </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200" baseline="0"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14603929484929"/>
+          <c:y val="0.193297579965348"/>
+          <c:w val="0.841233512212247"/>
+          <c:h val="0.616655635862998"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$126</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base (Seq.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$126:$K$126</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001569</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.003126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.013832</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.027681</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.138311</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.276646</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$127</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base (Par.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$127:$K$127</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000406</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000797</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.003473</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.006957</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.034645</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.069354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$128</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (Seq.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$128:$K$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.016906</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.082052</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.163856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$129</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (Par.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$129:$K$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.009623</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.046715</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.093163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$130</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goto (Seq.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$130:$K$130</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.019564</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.097194</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.194278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$131</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goto (Par.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$131:$K$131</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.019564</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.097196</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.194283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$132</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Orio (Seq.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$132:$K$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.96533107767952E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.04677677135099E-7</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.000102</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>0.000512</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>0.001024</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>0.007346</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.014979</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.074413</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.149929</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Orio (Par.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="10"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$K$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$133:$K$133</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.96533107767952E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.04677677135099E-7</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>6.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>0.000233</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>0.00046</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>0.002585</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>0.005396</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>0.023836</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>0.05293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="509087352"/>
+        <c:axId val="743991656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="509087352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="743991656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="50"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="743991656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509087352"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.240575379908722"/>
+          <c:y val="0.0452268934583943"/>
+          <c:w val="0.615506329113924"/>
+          <c:h val="0.126457707198289"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -3757,20 +4538,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>122174</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3786,21 +4569,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>85682</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>124461</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3817,20 +4602,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>48260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3846,21 +4633,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3876,21 +4665,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3899,6 +4690,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>85634</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3983,7 +4806,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Time (Sec.)</a:t>
           </a:r>
         </a:p>
@@ -3993,11 +4816,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.46697</cdr:x>
-      <cdr:y>0.89909</cdr:y>
+      <cdr:y>0.91319</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.62187</cdr:x>
-      <cdr:y>0.96961</cdr:y>
+      <cdr:y>0.98371</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4006,8 +4829,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2603500" y="3238500"/>
-          <a:ext cx="863600" cy="254000"/>
+          <a:off x="2603498" y="3289298"/>
+          <a:ext cx="863614" cy="254012"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4064,7 +4887,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Matrix Size</a:t>
           </a:r>
         </a:p>
@@ -4092,8 +4915,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-          <a:off x="-263525" y="1660525"/>
-          <a:ext cx="857250" cy="330200"/>
+          <a:off x="-263507" y="1660501"/>
+          <a:ext cx="857240" cy="330225"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4150,7 +4973,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Time (Sec.)</a:t>
           </a:r>
         </a:p>
@@ -4231,7 +5054,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Matrix Size</a:t>
           </a:r>
         </a:p>
@@ -4317,7 +5140,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Time (Sec.)</a:t>
           </a:r>
         </a:p>
@@ -4398,7 +5221,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Matrix Size</a:t>
           </a:r>
         </a:p>
@@ -4550,7 +5373,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Time (Sec.)</a:t>
           </a:r>
         </a:p>
@@ -4631,7 +5454,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Matrix Size</a:t>
           </a:r>
         </a:p>
@@ -4645,12 +5468,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.00618</cdr:x>
-      <cdr:y>0.38985</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.39213</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.04328</cdr:x>
-      <cdr:y>0.54084</cdr:y>
+      <cdr:x>0.05556</cdr:x>
+      <cdr:y>0.52662</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4659,8 +5482,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-          <a:off x="-184150" y="2235200"/>
-          <a:ext cx="774700" cy="304800"/>
+          <a:off x="-86611" y="1628420"/>
+          <a:ext cx="528825" cy="355603"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4671,7 +5494,7 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>MFLOP/s</a:t>
           </a:r>
         </a:p>
@@ -4680,12 +5503,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.47218</cdr:x>
-      <cdr:y>0.92946</cdr:y>
+      <cdr:x>0.4706</cdr:x>
+      <cdr:y>0.91918</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.56646</cdr:x>
-      <cdr:y>0.98886</cdr:y>
+      <cdr:x>0.56488</cdr:x>
+      <cdr:y>0.97858</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4694,8 +5517,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3879850" y="4768850"/>
-          <a:ext cx="774700" cy="304800"/>
+          <a:off x="3030160" y="3632809"/>
+          <a:ext cx="607059" cy="234763"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4770,8 +5593,175 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0"/>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Array Size</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.409</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.05923</cdr:x>
+      <cdr:y>0.64699</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-263525" y="1736725"/>
+          <a:ext cx="857250" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
+            <a:t>Time (Sec.)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.46697</cdr:x>
+      <cdr:y>0.92948</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.62187</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3724366" y="4717735"/>
+          <a:ext cx="1235420" cy="353533"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
+            <a:t>Matrix Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4789,11 +5779,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5343,7 +6333,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5598,19 +6587,22 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K116" sqref="K116"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" workbookViewId="0">
+      <selection activeCell="S105" sqref="S105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6991,8 +7983,244 @@
         <v>1511.44</v>
       </c>
     </row>
+    <row r="124" spans="1:11">
+      <c r="A124" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <v>100</v>
+      </c>
+      <c r="D125">
+        <v>1000</v>
+      </c>
+      <c r="E125">
+        <v>10000</v>
+      </c>
+      <c r="F125">
+        <v>50000</v>
+      </c>
+      <c r="G125">
+        <v>100000</v>
+      </c>
+      <c r="H125">
+        <v>500000</v>
+      </c>
+      <c r="I125">
+        <v>1000000</v>
+      </c>
+      <c r="J125">
+        <v>5000000</v>
+      </c>
+      <c r="K125">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C126" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D126" s="1">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="E126" s="1">
+        <v>3.2400000000000001E-4</v>
+      </c>
+      <c r="F126" s="1">
+        <v>1.5690000000000001E-3</v>
+      </c>
+      <c r="G126" s="1">
+        <v>3.1259999999999999E-3</v>
+      </c>
+      <c r="H126" s="1">
+        <v>1.3832000000000001E-2</v>
+      </c>
+      <c r="I126" s="1">
+        <v>2.7681000000000001E-2</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0.13831099999999999</v>
+      </c>
+      <c r="K126" s="1">
+        <v>0.276646</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C127" s="1">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="E127" s="1">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="F127" s="1">
+        <v>4.06E-4</v>
+      </c>
+      <c r="G127" s="1">
+        <v>7.9699999999999997E-4</v>
+      </c>
+      <c r="H127" s="1">
+        <v>3.473E-3</v>
+      </c>
+      <c r="I127" s="1">
+        <v>6.9569999999999996E-3</v>
+      </c>
+      <c r="J127" s="1">
+        <v>3.4645000000000002E-2</v>
+      </c>
+      <c r="K127" s="1">
+        <v>6.9353999999999999E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="I128" s="1">
+        <v>1.6906000000000001E-2</v>
+      </c>
+      <c r="J128" s="1">
+        <v>8.2052E-2</v>
+      </c>
+      <c r="K128" s="1">
+        <v>0.163856</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" t="s">
+        <v>21</v>
+      </c>
+      <c r="I129" s="1">
+        <v>9.6229999999999996E-3</v>
+      </c>
+      <c r="J129" s="1">
+        <v>4.6715E-2</v>
+      </c>
+      <c r="K129" s="1">
+        <v>9.3162999999999996E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" t="s">
+        <v>22</v>
+      </c>
+      <c r="I130" s="1">
+        <v>1.9564000000000002E-2</v>
+      </c>
+      <c r="J130" s="1">
+        <v>9.7194000000000003E-2</v>
+      </c>
+      <c r="K130" s="1">
+        <v>0.19427800000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
+      <c r="I131" s="1">
+        <v>1.9564000000000002E-2</v>
+      </c>
+      <c r="J131" s="1">
+        <v>9.7196000000000005E-2</v>
+      </c>
+      <c r="K131" s="1">
+        <v>0.19428300000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" t="s">
+        <v>24</v>
+      </c>
+      <c r="B132">
+        <f>20/6744609447</f>
+        <v>2.9653310776795226E-9</v>
+      </c>
+      <c r="C132">
+        <f>200/1910627036</f>
+        <v>1.0467767713509944E-7</v>
+      </c>
+      <c r="D132" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1.02E-4</v>
+      </c>
+      <c r="F132" s="1">
+        <v>5.1199999999999998E-4</v>
+      </c>
+      <c r="G132" s="1">
+        <v>1.024E-3</v>
+      </c>
+      <c r="H132" s="1">
+        <v>7.3460000000000001E-3</v>
+      </c>
+      <c r="I132" s="1">
+        <v>1.4978999999999999E-2</v>
+      </c>
+      <c r="J132" s="1">
+        <v>7.4413000000000007E-2</v>
+      </c>
+      <c r="K132" s="1">
+        <v>0.14992900000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" t="s">
+        <v>25</v>
+      </c>
+      <c r="B133">
+        <f>20/6744609447</f>
+        <v>2.9653310776795226E-9</v>
+      </c>
+      <c r="C133">
+        <f>200/1910627036</f>
+        <v>1.0467767713509944E-7</v>
+      </c>
+      <c r="D133" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="E133" s="1">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="F133" s="1">
+        <v>2.33E-4</v>
+      </c>
+      <c r="G133" s="1">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="H133" s="1">
+        <v>2.5850000000000001E-3</v>
+      </c>
+      <c r="I133" s="1">
+        <v>5.3959999999999998E-3</v>
+      </c>
+      <c r="J133" s="1">
+        <v>2.3836E-2</v>
+      </c>
+      <c r="K133" s="1">
+        <v>5.2929999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
made figures more readable (I hope)
git-svn-id: https://svn.mcs.anl.gov/repos/performance/orio@432 e7ad4b5f-b827-0410-872f-f7f4bc3d1efb
</commit_message>
<xml_diff>
--- a/doc/papers/iccs09/figures/experiments.xlsx
+++ b/doc/papers/iccs09/figures/experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="32660" windowHeight="20440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-2300" yWindow="-24460" windowWidth="32660" windowHeight="23940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>C from Matlab</t>
   </si>
@@ -126,19 +126,7 @@
     <t>Orio (Par.)</t>
   </si>
   <si>
-    <t>Orio (Par.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orio (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ATLAS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orio (Par.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -150,48 +138,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Orio (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BG/P (MFLOPS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base (Par.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESSL (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESSL (Par.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goto (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goto (Par.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orio (Seq.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orio (Par.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>BG/P (seconds)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (S)</t>
+  </si>
+  <si>
+    <t>Base (S)</t>
+  </si>
+  <si>
+    <t>ESSL (S)</t>
+  </si>
+  <si>
+    <t>Goto (S)</t>
+  </si>
+  <si>
+    <t>Orio (P)</t>
+  </si>
+  <si>
+    <t>Base (P)</t>
+  </si>
+  <si>
+    <t>ESSL (P)</t>
+  </si>
+  <si>
+    <t>Goto (P)</t>
   </si>
 </sst>
 </file>
@@ -265,8 +241,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.109824224705397"/>
-          <c:y val="0.203430674402425"/>
+          <c:x val="0.111803698231308"/>
+          <c:y val="0.180994851605088"/>
           <c:w val="0.865118827686403"/>
           <c:h val="0.614879507736591"/>
         </c:manualLayout>
@@ -287,6 +263,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -375,11 +362,22 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
+                  <c:v>Orio (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -468,11 +466,15 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -566,6 +568,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -659,6 +672,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -752,6 +776,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F79646">
+                  <a:shade val="76000"/>
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$K$2</c:f>
@@ -832,11 +868,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="528458312"/>
-        <c:axId val="528461480"/>
+        <c:axId val="546550216"/>
+        <c:axId val="546553528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="528458312"/>
+        <c:axId val="546550216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,14 +892,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528461480"/>
+        <c:crossAx val="546553528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="528461480"/>
+        <c:axId val="546553528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528458312"/>
+        <c:crossAx val="546550216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -935,8 +971,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110077843344753"/>
-          <c:y val="0.167427218149455"/>
+          <c:x val="0.106143869604812"/>
+          <c:y val="0.16742731677771"/>
           <c:w val="0.862489552131724"/>
           <c:h val="0.664745147476466"/>
         </c:manualLayout>
@@ -957,6 +993,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1045,11 +1092,22 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
+                  <c:v>Orio (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1138,11 +1196,15 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1236,6 +1298,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1329,6 +1402,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1422,6 +1506,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F79646">
+                  <a:shade val="76000"/>
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$25:$K$25</c:f>
@@ -1502,11 +1598,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="656502760"/>
-        <c:axId val="656505928"/>
+        <c:axId val="547136584"/>
+        <c:axId val="547515688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="656502760"/>
+        <c:axId val="547136584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1614,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400">
+              <a:defRPr sz="1600">
                 <a:latin typeface="Arial Narrow"/>
                 <a:cs typeface="Arial Narrow"/>
               </a:defRPr>
@@ -1526,14 +1622,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656505928"/>
+        <c:crossAx val="547515688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="656505928"/>
+        <c:axId val="547515688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656502760"/>
+        <c:crossAx val="547136584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1576,7 +1672,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1715,7 +1811,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
+                  <c:v>Orio (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1808,7 +1904,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2172,11 +2268,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="656576328"/>
-        <c:axId val="656564232"/>
+        <c:axId val="546796488"/>
+        <c:axId val="547081144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="656576328"/>
+        <c:axId val="546796488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,14 +2292,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656564232"/>
+        <c:crossAx val="547081144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="656564232"/>
+        <c:axId val="547081144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656576328"/>
+        <c:crossAx val="546796488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2246,7 +2342,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -2277,8 +2373,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.114373120973515"/>
           <c:y val="0.167427218149455"/>
-          <c:w val="0.858026843235505"/>
-          <c:h val="0.674955074634076"/>
+          <c:w val="0.86394399664539"/>
+          <c:h val="0.665339693115284"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2297,6 +2393,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2385,11 +2492,22 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
+                  <c:v>Orio (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2478,11 +2596,15 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2563,8 +2685,226 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel MKL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$K$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$73:$K$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0518</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.276</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.619</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ATLAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F79646">
+                  <a:shade val="76000"/>
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="F79646">
+                    <a:shade val="76000"/>
+                    <a:shade val="95000"/>
+                    <a:satMod val="105000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$K$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$74:$K$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.00935</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.835</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$72</c:f>
@@ -2576,6 +2916,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$68:$K$68</c:f>
@@ -2655,198 +3006,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$73</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Intel MKL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$68:$K$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18000.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$73:$K$73</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0518</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0684</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.154</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.276</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.431</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.619</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.845</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.39</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.73</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$74</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ATLAS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$68:$K$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18000.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$74:$K$74</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.00935</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0418</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.316</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.556</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.835</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.51</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="656621240"/>
-        <c:axId val="656624568"/>
+        <c:axId val="69874920"/>
+        <c:axId val="525277528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="656621240"/>
+        <c:axId val="69874920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2858,7 +3023,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400">
+              <a:defRPr sz="1600">
                 <a:latin typeface="Arial Narrow"/>
                 <a:cs typeface="Arial Narrow"/>
               </a:defRPr>
@@ -2866,14 +3031,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656624568"/>
+        <c:crossAx val="525277528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="656624568"/>
+        <c:axId val="525277528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,7 +3051,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400">
+              <a:defRPr sz="1600">
                 <a:latin typeface="Arial Narrow"/>
                 <a:cs typeface="Arial Narrow"/>
               </a:defRPr>
@@ -2894,7 +3059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656621240"/>
+        <c:crossAx val="69874920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2916,7 +3081,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -2945,10 +3110,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.137919010123735"/>
+          <c:x val="0.155612075196531"/>
           <c:y val="0.0263381928744055"/>
-          <c:w val="0.820822084739407"/>
-          <c:h val="0.741538485014954"/>
+          <c:w val="0.803128977785169"/>
+          <c:h val="0.78102441937168"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2962,500 +3127,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Base (Seq.)</c:v>
+                  <c:v>Base (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="10"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$103:$K$103</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>69.204658</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>221.72</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>364.54</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>247.19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>254.94</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>255.88</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>289.18</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>289.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>289.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>289.18</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$104</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Base (Par.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$104:$K$104</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>15.14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>122.53</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>695.77</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>834.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>984.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1003.73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1151.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1150.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1154.57</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1153.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$105</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ESSL (Seq.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$105:$K$105</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="7">
-                  <c:v>473.21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>487.49</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>488.23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$106</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ESSL (Par.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$106:$K$106</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="7">
-                  <c:v>831.3099999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>856.25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>858.71</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$107</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Goto (Seq.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$107:$K$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="7">
-                  <c:v>408.91</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>411.55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>411.78</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$108</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Goto (Par.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$102:$K$102</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$108:$K$108</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="7">
-                  <c:v>408.91</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>411.54</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>411.77</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$109</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="plus"/>
             <c:size val="10"/>
             <c:spPr>
               <a:ln>
@@ -3472,34 +3150,564 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10.0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$103:$K$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>69.204658</c:v>
+                </c:pt>
                 <c:pt idx="1">
+                  <c:v>221.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>364.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247.19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>254.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>255.88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>289.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>289.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>289.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>289.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>100.0</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$104:$K$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122.53</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>695.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>834.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>984.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1003.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1151.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1150.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1154.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1153.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$106</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1000.0</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$106:$K$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>831.3099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>856.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>858.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goto (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
                 <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>10000.0</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$107:$K$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>408.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>411.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>411.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$108</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goto (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F79646">
+                  <a:shade val="76000"/>
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100000.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500000.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$108:$K$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>408.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>411.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>411.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$105</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$105:$K$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>473.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>487.49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$109</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Orio (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$102:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3553,7 +3761,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3576,34 +3784,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>100.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1000.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3649,11 +3857,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="656689256"/>
-        <c:axId val="656694264"/>
+        <c:axId val="546386872"/>
+        <c:axId val="547396024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="656689256"/>
+        <c:axId val="546386872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,7 +3873,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0">
+              <a:defRPr sz="1600" b="0">
                 <a:latin typeface="Arial Narrow"/>
                 <a:cs typeface="Arial Narrow"/>
               </a:defRPr>
@@ -3673,14 +3881,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656694264"/>
+        <c:crossAx val="547396024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="656694264"/>
+        <c:axId val="547396024"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3696,7 +3904,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0">
+              <a:defRPr sz="1600" b="0" spc="-120">
                 <a:latin typeface="Arial Narrow"/>
                 <a:cs typeface="Arial Narrow"/>
               </a:defRPr>
@@ -3704,7 +3912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="656689256"/>
+        <c:crossAx val="546386872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3715,10 +3923,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.533926696662917"/>
-          <c:y val="0.518260544466825"/>
-          <c:w val="0.404533704925215"/>
-          <c:h val="0.228952989787168"/>
+          <c:x val="0.441224588050754"/>
+          <c:y val="0.466846648988928"/>
+          <c:w val="0.497235863268571"/>
+          <c:h val="0.280366829949598"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3726,7 +3934,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800">
+              <a:latin typeface="Arial Narrow"/>
+              <a:cs typeface="Arial Narrow"/>
+            </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -3781,7 +3992,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Base (Seq.)</c:v>
+                  <c:v>Base (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3874,7 +4085,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Base (Par.)</c:v>
+                  <c:v>Base (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3967,7 +4178,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ESSL (Seq.)</c:v>
+                  <c:v>ESSL (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4039,7 +4250,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ESSL (Par.)</c:v>
+                  <c:v>ESSL (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4111,7 +4322,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Goto (Seq.)</c:v>
+                  <c:v>Goto (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4183,7 +4394,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Goto (Par.)</c:v>
+                  <c:v>Goto (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4255,7 +4466,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Seq.)</c:v>
+                  <c:v>Orio (S)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4352,7 +4563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Orio (Par.)</c:v>
+                  <c:v>Orio (P)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4441,11 +4652,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="509087352"/>
-        <c:axId val="743991656"/>
+        <c:axId val="547143336"/>
+        <c:axId val="546888584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="509087352"/>
+        <c:axId val="547143336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4465,7 +4676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="743991656"/>
+        <c:crossAx val="546888584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4474,7 +4685,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="743991656"/>
+        <c:axId val="546888584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4495,7 +4706,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509087352"/>
+        <c:crossAx val="547143336"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -4516,7 +4728,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4538,15 +4750,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:colOff>937260</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4663,19 +4875,14 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
       <xdr:row>92</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="6253480" cy="3838428"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6"/>
@@ -4693,20 +4900,20 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>193040</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>96520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>85634</xdr:rowOff>
+      <xdr:colOff>853440</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>156754</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4806,8 +5013,12 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Time (Sec.)</a:t>
+            <a:t> (Sec.)</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4887,8 +5098,14 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>Matrix</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Matrix Size</a:t>
+            <a:t> Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4915,8 +5132,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-          <a:off x="-263507" y="1660501"/>
-          <a:ext cx="857240" cy="330225"/>
+          <a:off x="-257923" y="1721792"/>
+          <a:ext cx="898276" cy="382429"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4973,7 +5190,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1600" b="0"/>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
             <a:t>Time (Sec.)</a:t>
           </a:r>
         </a:p>
@@ -5054,8 +5271,16 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Matrix</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Matrix Size</a:t>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5383,11 +5608,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.47045</cdr:x>
-      <cdr:y>0.92638</cdr:y>
+      <cdr:y>0.91612</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.625</cdr:x>
-      <cdr:y>0.98773</cdr:y>
+      <cdr:y>0.97747</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5396,8 +5621,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2628900" y="3835400"/>
-          <a:ext cx="863600" cy="254000"/>
+          <a:off x="3029181" y="3630048"/>
+          <a:ext cx="995132" cy="243093"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5454,8 +5679,12 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Matrix</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Matrix Size</a:t>
+            <a:t> Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5469,11 +5698,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0</cdr:x>
-      <cdr:y>0.39213</cdr:y>
+      <cdr:y>0.35067</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.05556</cdr:x>
-      <cdr:y>0.52662</cdr:y>
+      <cdr:y>0.52042</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5482,8 +5711,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-          <a:off x="-86611" y="1628420"/>
-          <a:ext cx="528825" cy="355603"/>
+          <a:off x="-156576" y="1542511"/>
+          <a:ext cx="670897" cy="357745"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5494,8 +5723,12 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>MFLOP</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>MFLOP/s</a:t>
+            <a:t>/s</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5503,12 +5736,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.4706</cdr:x>
-      <cdr:y>0.91918</cdr:y>
+      <cdr:x>0.42998</cdr:x>
+      <cdr:y>0.90414</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.56488</cdr:x>
-      <cdr:y>0.97858</cdr:y>
+      <cdr:x>0.52426</cdr:x>
+      <cdr:y>0.96354</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5517,8 +5750,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3030160" y="3632809"/>
-          <a:ext cx="607059" cy="234763"/>
+          <a:off x="2688887" y="3470465"/>
+          <a:ext cx="589579" cy="228002"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5594,8 +5827,17 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Array Size</a:t>
+            <a:t>Array </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Size (x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" baseline="0"/>
+            <a:t> 1,000)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -5679,8 +5921,12 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Time (Sec.)</a:t>
+            <a:t> (Sec.)</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5761,7 +6007,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t>Matrix Size</a:t>
+            <a:t>Matrix </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5779,11 +6029,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6333,6 +6583,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6589,8 +6840,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" workbookViewId="0">
-      <selection activeCell="S105" sqref="S105"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6679,7 +6930,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>2.9000000000000001E-2</v>
@@ -6714,7 +6965,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>3.6999999999999998E-2</v>
@@ -6926,7 +7177,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B27">
         <v>8.9999999999999993E-3</v>
@@ -6961,7 +7212,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>9.4E-2</v>
@@ -7173,7 +7424,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B48">
         <v>1.7000000000000001E-2</v>
@@ -7208,7 +7459,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B49">
         <v>1.0999999999999999E-2</v>
@@ -7313,7 +7564,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1">
         <v>5.3600000000000002E-5</v>
@@ -7348,7 +7599,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -7420,7 +7671,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>1.2E-2</v>
@@ -7455,7 +7706,7 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B71">
         <v>8.9999999999999993E-3</v>
@@ -7632,17 +7883,17 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -7752,44 +8003,44 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="B102">
+        <v>0.01</v>
+      </c>
+      <c r="C102">
+        <v>0.1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
         <v>10</v>
       </c>
-      <c r="C102">
+      <c r="F102">
+        <v>50</v>
+      </c>
+      <c r="G102">
         <v>100</v>
       </c>
-      <c r="D102">
+      <c r="H102">
+        <v>500</v>
+      </c>
+      <c r="I102">
         <v>1000</v>
       </c>
-      <c r="E102">
+      <c r="J102">
+        <v>5000</v>
+      </c>
+      <c r="K102">
         <v>10000</v>
-      </c>
-      <c r="F102">
-        <v>50000</v>
-      </c>
-      <c r="G102">
-        <v>100000</v>
-      </c>
-      <c r="H102">
-        <v>500000</v>
-      </c>
-      <c r="I102">
-        <v>1000000</v>
-      </c>
-      <c r="J102">
-        <v>5000000</v>
-      </c>
-      <c r="K102">
-        <v>10000000</v>
       </c>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B103">
         <v>69.204657999999995</v>
@@ -7824,7 +8075,7 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B104">
         <v>15.14</v>
@@ -7859,7 +8110,7 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I105">
         <v>473.21</v>
@@ -7887,7 +8138,7 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I107">
         <v>408.91</v>
@@ -7901,7 +8152,7 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I108">
         <v>408.91</v>
@@ -7915,7 +8166,7 @@
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B109">
         <v>6744.61</v>
@@ -7950,7 +8201,7 @@
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B110">
         <v>6739.19</v>
@@ -7985,7 +8236,7 @@
     </row>
     <row r="124" spans="1:11">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -8022,7 +8273,7 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B126" s="1">
         <v>9.9999999999999995E-7</v>
@@ -8057,7 +8308,7 @@
     </row>
     <row r="127" spans="1:11">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B127" s="1">
         <v>5.0000000000000004E-6</v>
@@ -8092,7 +8343,7 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I128" s="1">
         <v>1.6906000000000001E-2</v>
@@ -8120,7 +8371,7 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I130" s="1">
         <v>1.9564000000000002E-2</v>
@@ -8134,7 +8385,7 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I131" s="1">
         <v>1.9564000000000002E-2</v>
@@ -8148,7 +8399,7 @@
     </row>
     <row r="132" spans="1:11">
       <c r="A132" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B132">
         <f>20/6744609447</f>
@@ -8185,7 +8436,7 @@
     </row>
     <row r="133" spans="1:11">
       <c r="A133" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B133">
         <f>20/6744609447</f>
@@ -8223,7 +8474,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Final changes to address reviewer comments (mainly Reviewer 3)
git-svn-id: https://svn.mcs.anl.gov/repos/performance/orio@441 e7ad4b5f-b827-0410-872f-f7f4bc3d1efb
</commit_message>
<xml_diff>
--- a/doc/papers/iccs09/figures/experiments.xlsx
+++ b/doc/papers/iccs09/figures/experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-2300" yWindow="-24460" windowWidth="32660" windowHeight="23940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="32660" windowHeight="20560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>C from Matlab</t>
   </si>
@@ -168,6 +168,14 @@
   </si>
   <si>
     <t>Goto (P)</t>
+  </si>
+  <si>
+    <t>SPLIT into two parts:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goto (S&amp;P)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -931,8 +939,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.132295123132387"/>
-          <c:y val="0.0350938124483963"/>
+          <c:x val="0.148130466767664"/>
+          <c:y val="0.0254784978800727"/>
           <c:w val="0.812401843846968"/>
           <c:h val="0.151329532084352"/>
         </c:manualLayout>
@@ -942,7 +950,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4729,6 +4737,569 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.187475608007431"/>
+          <c:y val="0.197020492630729"/>
+          <c:w val="0.812524391992569"/>
+          <c:h val="0.618084746618211"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$147:$E$147</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.003126</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.013832</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.027681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.138311</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$148</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$148:$E$148</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.000797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.003473</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.006957</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.034645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$149</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$149:$E$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>0.016906</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.082052</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$150</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ESSL (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$150:$E$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>0.009623</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.046715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goto (S&amp;P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$151:$E$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>0.019564</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.097194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$152</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Orio (S)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:ln w="19050" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$152:$E$152</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.001024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.007346</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.014979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.074413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$153</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Orio (P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$146:$E$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$153:$E$153</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.00046</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.002585</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.005396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.023836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="544318280"/>
+        <c:axId val="542015256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="544318280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="542015256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="542015256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600">
+                <a:latin typeface="Arial Narrow"/>
+                <a:cs typeface="Arial Narrow"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544318280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.195636405009944"/>
+          <c:y val="0.0158631132646881"/>
+          <c:w val="0.801870935966733"/>
+          <c:h val="0.173047143145568"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" spc="-100"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4904,16 +5475,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>193040</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>111760</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>157480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>853440</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>156754</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>629920</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>55154</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4929,6 +5500,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>386080</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5105,7 +5708,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
-            <a:t> Size</a:t>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Size</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -6008,6 +6615,187 @@
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="0"/>
             <a:t>Matrix </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Size</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.39362</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.05923</cdr:x>
+      <cdr:y>0.63161</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-281495" y="1841157"/>
+          <a:ext cx="943011" cy="380022"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0"/>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
+            <a:t> (Sec.)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.46697</cdr:x>
+      <cdr:y>0.91319</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.62187</cdr:x>
+      <cdr:y>0.98371</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2603498" y="3289298"/>
+          <a:ext cx="863614" cy="254012"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>Array</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0"/>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" b="0"/>
@@ -6583,7 +7371,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6838,10 +7625,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H152" sqref="H152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8471,9 +9258,257 @@
         <v>5.2929999999999998E-2</v>
       </c>
     </row>
+    <row r="135" spans="1:11">
+      <c r="A135" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="B138">
+        <v>10</v>
+      </c>
+      <c r="C138">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>1000</v>
+      </c>
+      <c r="E138">
+        <v>10000</v>
+      </c>
+      <c r="F138">
+        <v>50000</v>
+      </c>
+      <c r="G138">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" t="s">
+        <v>16</v>
+      </c>
+      <c r="B139" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C139" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D139" s="1">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="E139" s="1">
+        <v>3.2400000000000001E-4</v>
+      </c>
+      <c r="F139" s="1">
+        <v>1.5690000000000001E-3</v>
+      </c>
+      <c r="G139" s="1">
+        <v>3.1259999999999999E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" t="s">
+        <v>20</v>
+      </c>
+      <c r="B140" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C140" s="1">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="D140" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="E140" s="1">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="F140" s="1">
+        <v>4.06E-4</v>
+      </c>
+      <c r="G140" s="1">
+        <v>7.9699999999999997E-4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" t="s">
+        <v>15</v>
+      </c>
+      <c r="B141">
+        <f>20/6744609447</f>
+        <v>2.9653310776795226E-9</v>
+      </c>
+      <c r="C141">
+        <f>200/1910627036</f>
+        <v>1.0467767713509944E-7</v>
+      </c>
+      <c r="D141" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1.02E-4</v>
+      </c>
+      <c r="F141" s="1">
+        <v>5.1199999999999998E-4</v>
+      </c>
+      <c r="G141" s="1">
+        <v>1.024E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" t="s">
+        <v>19</v>
+      </c>
+      <c r="B142">
+        <f>20/6744609447</f>
+        <v>2.9653310776795226E-9</v>
+      </c>
+      <c r="C142">
+        <f>200/1910627036</f>
+        <v>1.0467767713509944E-7</v>
+      </c>
+      <c r="D142" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="E142" s="1">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="F142" s="1">
+        <v>2.33E-4</v>
+      </c>
+      <c r="G142" s="1">
+        <v>4.6000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="B146">
+        <v>100000</v>
+      </c>
+      <c r="C146">
+        <v>500000</v>
+      </c>
+      <c r="D146">
+        <v>1000000</v>
+      </c>
+      <c r="E146">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>16</v>
+      </c>
+      <c r="B147" s="1">
+        <v>3.1259999999999999E-3</v>
+      </c>
+      <c r="C147" s="1">
+        <v>1.3832000000000001E-2</v>
+      </c>
+      <c r="D147" s="1">
+        <v>2.7681000000000001E-2</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0.13831099999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>20</v>
+      </c>
+      <c r="B148" s="1">
+        <v>7.9699999999999997E-4</v>
+      </c>
+      <c r="C148" s="1">
+        <v>3.473E-3</v>
+      </c>
+      <c r="D148" s="1">
+        <v>6.9569999999999996E-3</v>
+      </c>
+      <c r="E148" s="1">
+        <v>3.4645000000000002E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>17</v>
+      </c>
+      <c r="D149" s="1">
+        <v>1.6906000000000001E-2</v>
+      </c>
+      <c r="E149" s="1">
+        <v>8.2052E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150" s="1">
+        <v>9.6229999999999996E-3</v>
+      </c>
+      <c r="E150" s="1">
+        <v>4.6715E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>24</v>
+      </c>
+      <c r="D151" s="1">
+        <v>1.9564000000000002E-2</v>
+      </c>
+      <c r="E151" s="1">
+        <v>9.7194000000000003E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>15</v>
+      </c>
+      <c r="B152" s="1">
+        <v>1.024E-3</v>
+      </c>
+      <c r="C152" s="1">
+        <v>7.3460000000000001E-3</v>
+      </c>
+      <c r="D152" s="1">
+        <v>1.4978999999999999E-2</v>
+      </c>
+      <c r="E152" s="1">
+        <v>7.4413000000000007E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>19</v>
+      </c>
+      <c r="B153" s="1">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="C153" s="1">
+        <v>2.5850000000000001E-3</v>
+      </c>
+      <c r="D153" s="1">
+        <v>5.3959999999999998E-3</v>
+      </c>
+      <c r="E153" s="1">
+        <v>2.3836E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>